<commit_message>
adding prefiring monitoring seed
</commit_message>
<xml_diff>
--- a/development/L1Menu_Collisions2022_v1_1_0/PrescaleTable/L1Menu_Collisions2022_v1_1_0.xlsx
+++ b/development/L1Menu_Collisions2022_v1_1_0/PrescaleTable/L1Menu_Collisions2022_v1_1_0.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K391"/>
+  <dimension ref="A1:K392"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13627,11 +13627,11 @@
     </row>
     <row r="357">
       <c r="A357" t="n">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B357" t="inlineStr">
         <is>
-          <t>L1_NotBptxOR</t>
+          <t>L1_MinimumBiasHF0</t>
         </is>
       </c>
       <c r="C357" t="n">
@@ -13664,11 +13664,11 @@
     </row>
     <row r="358">
       <c r="A358" t="n">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B358" t="inlineStr">
         <is>
-          <t>L1_BptxOR</t>
+          <t>L1_NotBptxOR</t>
         </is>
       </c>
       <c r="C358" t="n">
@@ -13701,11 +13701,11 @@
     </row>
     <row r="359">
       <c r="A359" t="n">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B359" t="inlineStr">
         <is>
-          <t>L1_BptxXOR</t>
+          <t>L1_BptxOR</t>
         </is>
       </c>
       <c r="C359" t="n">
@@ -13738,11 +13738,11 @@
     </row>
     <row r="360">
       <c r="A360" t="n">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B360" t="inlineStr">
         <is>
-          <t>L1_BptxPlus</t>
+          <t>L1_BptxXOR</t>
         </is>
       </c>
       <c r="C360" t="n">
@@ -13775,11 +13775,11 @@
     </row>
     <row r="361">
       <c r="A361" t="n">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B361" t="inlineStr">
         <is>
-          <t>L1_BptxMinus</t>
+          <t>L1_BptxPlus</t>
         </is>
       </c>
       <c r="C361" t="n">
@@ -13812,11 +13812,11 @@
     </row>
     <row r="362">
       <c r="A362" t="n">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B362" t="inlineStr">
         <is>
-          <t>L1_UnpairedBunchBptxPlus</t>
+          <t>L1_BptxMinus</t>
         </is>
       </c>
       <c r="C362" t="n">
@@ -13849,11 +13849,11 @@
     </row>
     <row r="363">
       <c r="A363" t="n">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B363" t="inlineStr">
         <is>
-          <t>L1_UnpairedBunchBptxMinus</t>
+          <t>L1_UnpairedBunchBptxPlus</t>
         </is>
       </c>
       <c r="C363" t="n">
@@ -13886,85 +13886,85 @@
     </row>
     <row r="364">
       <c r="A364" t="n">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="B364" t="inlineStr">
         <is>
-          <t>L1_IsolatedBunch</t>
+          <t>L1_UnpairedBunchBptxMinus</t>
         </is>
       </c>
       <c r="C364" t="n">
         <v>0</v>
       </c>
       <c r="D364" t="n">
-        <v>110</v>
+        <v>0</v>
       </c>
       <c r="E364" t="n">
-        <v>110</v>
+        <v>0</v>
       </c>
       <c r="F364" t="n">
-        <v>110</v>
+        <v>0</v>
       </c>
       <c r="G364" t="n">
-        <v>110</v>
+        <v>0</v>
       </c>
       <c r="H364" t="n">
-        <v>110</v>
+        <v>0</v>
       </c>
       <c r="I364" t="n">
-        <v>110</v>
+        <v>0</v>
       </c>
       <c r="J364" t="n">
-        <v>110</v>
+        <v>0</v>
       </c>
       <c r="K364" t="n">
-        <v>110</v>
+        <v>0</v>
       </c>
     </row>
     <row r="365">
       <c r="A365" t="n">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B365" t="inlineStr">
         <is>
-          <t>L1_FirstBunchBeforeTrain</t>
+          <t>L1_IsolatedBunch</t>
         </is>
       </c>
       <c r="C365" t="n">
         <v>0</v>
       </c>
       <c r="D365" t="n">
-        <v>269167</v>
+        <v>110</v>
       </c>
       <c r="E365" t="n">
-        <v>269167</v>
+        <v>110</v>
       </c>
       <c r="F365" t="n">
-        <v>269167</v>
+        <v>110</v>
       </c>
       <c r="G365" t="n">
-        <v>269167</v>
+        <v>110</v>
       </c>
       <c r="H365" t="n">
-        <v>269167</v>
+        <v>110</v>
       </c>
       <c r="I365" t="n">
-        <v>269167</v>
+        <v>110</v>
       </c>
       <c r="J365" t="n">
-        <v>269167</v>
+        <v>110</v>
       </c>
       <c r="K365" t="n">
-        <v>269167</v>
+        <v>110</v>
       </c>
     </row>
     <row r="366">
       <c r="A366" t="n">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B366" t="inlineStr">
         <is>
-          <t>L1_FirstBunchInTrain</t>
+          <t>L1_FirstBunchBeforeTrain</t>
         </is>
       </c>
       <c r="C366" t="n">
@@ -13997,48 +13997,48 @@
     </row>
     <row r="367">
       <c r="A367" t="n">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B367" t="inlineStr">
         <is>
-          <t>L1_SecondBunchInTrain</t>
+          <t>L1_FirstBunchInTrain</t>
         </is>
       </c>
       <c r="C367" t="n">
         <v>0</v>
       </c>
       <c r="D367" t="n">
-        <v>0</v>
+        <v>269167</v>
       </c>
       <c r="E367" t="n">
-        <v>0</v>
+        <v>269167</v>
       </c>
       <c r="F367" t="n">
-        <v>0</v>
+        <v>269167</v>
       </c>
       <c r="G367" t="n">
-        <v>0</v>
+        <v>269167</v>
       </c>
       <c r="H367" t="n">
-        <v>0</v>
+        <v>269167</v>
       </c>
       <c r="I367" t="n">
-        <v>0</v>
+        <v>269167</v>
       </c>
       <c r="J367" t="n">
-        <v>0</v>
+        <v>269167</v>
       </c>
       <c r="K367" t="n">
-        <v>0</v>
+        <v>269167</v>
       </c>
     </row>
     <row r="368">
       <c r="A368" t="n">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B368" t="inlineStr">
         <is>
-          <t>L1_SecondLastBunchInTrain</t>
+          <t>L1_SecondBunchInTrain</t>
         </is>
       </c>
       <c r="C368" t="n">
@@ -14071,11 +14071,11 @@
     </row>
     <row r="369">
       <c r="A369" t="n">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B369" t="inlineStr">
         <is>
-          <t>L1_LastBunchInTrain</t>
+          <t>L1_SecondLastBunchInTrain</t>
         </is>
       </c>
       <c r="C369" t="n">
@@ -14108,48 +14108,48 @@
     </row>
     <row r="370">
       <c r="A370" t="n">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B370" t="inlineStr">
         <is>
-          <t>L1_FirstBunchAfterTrain</t>
+          <t>L1_LastBunchInTrain</t>
         </is>
       </c>
       <c r="C370" t="n">
         <v>0</v>
       </c>
       <c r="D370" t="n">
-        <v>269167</v>
+        <v>0</v>
       </c>
       <c r="E370" t="n">
-        <v>269167</v>
+        <v>0</v>
       </c>
       <c r="F370" t="n">
-        <v>269167</v>
+        <v>0</v>
       </c>
       <c r="G370" t="n">
-        <v>269167</v>
+        <v>0</v>
       </c>
       <c r="H370" t="n">
-        <v>269167</v>
+        <v>0</v>
       </c>
       <c r="I370" t="n">
-        <v>269167</v>
+        <v>0</v>
       </c>
       <c r="J370" t="n">
-        <v>269167</v>
+        <v>0</v>
       </c>
       <c r="K370" t="n">
-        <v>269167</v>
+        <v>0</v>
       </c>
     </row>
     <row r="371">
       <c r="A371" t="n">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B371" t="inlineStr">
         <is>
-          <t>L1_LastCollisionInTrain</t>
+          <t>L1_FirstBunchAfterTrain</t>
         </is>
       </c>
       <c r="C371" t="n">
@@ -14182,11 +14182,11 @@
     </row>
     <row r="372">
       <c r="A372" t="n">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B372" t="inlineStr">
         <is>
-          <t>L1_FirstCollisionInTrain</t>
+          <t>L1_LastCollisionInTrain</t>
         </is>
       </c>
       <c r="C372" t="n">
@@ -14219,85 +14219,85 @@
     </row>
     <row r="373">
       <c r="A373" t="n">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B373" t="inlineStr">
         <is>
-          <t>L1_FirstCollisionInOrbit</t>
+          <t>L1_FirstCollisionInTrain</t>
         </is>
       </c>
       <c r="C373" t="n">
         <v>0</v>
       </c>
       <c r="D373" t="n">
-        <v>1103</v>
+        <v>269167</v>
       </c>
       <c r="E373" t="n">
-        <v>1103</v>
+        <v>269167</v>
       </c>
       <c r="F373" t="n">
-        <v>1103</v>
+        <v>269167</v>
       </c>
       <c r="G373" t="n">
-        <v>1103</v>
+        <v>269167</v>
       </c>
       <c r="H373" t="n">
-        <v>1103</v>
+        <v>269167</v>
       </c>
       <c r="I373" t="n">
-        <v>1103</v>
+        <v>269167</v>
       </c>
       <c r="J373" t="n">
-        <v>1103</v>
+        <v>269167</v>
       </c>
       <c r="K373" t="n">
-        <v>1103</v>
+        <v>269167</v>
       </c>
     </row>
     <row r="374">
       <c r="A374" t="n">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="B374" t="inlineStr">
         <is>
-          <t>L1_BPTX_NotOR_VME</t>
+          <t>L1_FirstCollisionInOrbit</t>
         </is>
       </c>
       <c r="C374" t="n">
         <v>0</v>
       </c>
       <c r="D374" t="n">
-        <v>0</v>
+        <v>1103</v>
       </c>
       <c r="E374" t="n">
-        <v>0</v>
+        <v>1103</v>
       </c>
       <c r="F374" t="n">
-        <v>0</v>
+        <v>1103</v>
       </c>
       <c r="G374" t="n">
-        <v>0</v>
+        <v>1103</v>
       </c>
       <c r="H374" t="n">
-        <v>0</v>
+        <v>1103</v>
       </c>
       <c r="I374" t="n">
-        <v>0</v>
+        <v>1103</v>
       </c>
       <c r="J374" t="n">
-        <v>0</v>
+        <v>1103</v>
       </c>
       <c r="K374" t="n">
-        <v>0</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="375">
       <c r="A375" t="n">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B375" t="inlineStr">
         <is>
-          <t>L1_BPTX_OR_Ref3_VME</t>
+          <t>L1_BPTX_NotOR_VME</t>
         </is>
       </c>
       <c r="C375" t="n">
@@ -14330,11 +14330,11 @@
     </row>
     <row r="376">
       <c r="A376" t="n">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="B376" t="inlineStr">
         <is>
-          <t>L1_BPTX_OR_Ref4_VME</t>
+          <t>L1_BPTX_OR_Ref3_VME</t>
         </is>
       </c>
       <c r="C376" t="n">
@@ -14367,11 +14367,11 @@
     </row>
     <row r="377">
       <c r="A377" t="n">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="B377" t="inlineStr">
         <is>
-          <t>L1_BPTX_RefAND_VME</t>
+          <t>L1_BPTX_OR_Ref4_VME</t>
         </is>
       </c>
       <c r="C377" t="n">
@@ -14404,11 +14404,11 @@
     </row>
     <row r="378">
       <c r="A378" t="n">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B378" t="inlineStr">
         <is>
-          <t>L1_BPTX_AND_Ref1_VME</t>
+          <t>L1_BPTX_RefAND_VME</t>
         </is>
       </c>
       <c r="C378" t="n">
@@ -14441,11 +14441,11 @@
     </row>
     <row r="379">
       <c r="A379" t="n">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B379" t="inlineStr">
         <is>
-          <t>L1_BPTX_AND_Ref3_VME</t>
+          <t>L1_BPTX_AND_Ref1_VME</t>
         </is>
       </c>
       <c r="C379" t="n">
@@ -14478,11 +14478,11 @@
     </row>
     <row r="380">
       <c r="A380" t="n">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B380" t="inlineStr">
         <is>
-          <t>L1_BPTX_AND_Ref4_VME</t>
+          <t>L1_BPTX_AND_Ref3_VME</t>
         </is>
       </c>
       <c r="C380" t="n">
@@ -14515,11 +14515,11 @@
     </row>
     <row r="381">
       <c r="A381" t="n">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B381" t="inlineStr">
         <is>
-          <t>L1_BPTX_BeamGas_Ref1_VME</t>
+          <t>L1_BPTX_AND_Ref4_VME</t>
         </is>
       </c>
       <c r="C381" t="n">
@@ -14552,11 +14552,11 @@
     </row>
     <row r="382">
       <c r="A382" t="n">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B382" t="inlineStr">
         <is>
-          <t>L1_BPTX_BeamGas_Ref2_VME</t>
+          <t>L1_BPTX_BeamGas_Ref1_VME</t>
         </is>
       </c>
       <c r="C382" t="n">
@@ -14589,11 +14589,11 @@
     </row>
     <row r="383">
       <c r="A383" t="n">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="B383" t="inlineStr">
         <is>
-          <t>L1_BPTX_BeamGas_B1_VME</t>
+          <t>L1_BPTX_BeamGas_Ref2_VME</t>
         </is>
       </c>
       <c r="C383" t="n">
@@ -14626,11 +14626,11 @@
     </row>
     <row r="384">
       <c r="A384" t="n">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="B384" t="inlineStr">
         <is>
-          <t>L1_BPTX_BeamGas_B2_VME</t>
+          <t>L1_BPTX_BeamGas_B1_VME</t>
         </is>
       </c>
       <c r="C384" t="n">
@@ -14663,85 +14663,85 @@
     </row>
     <row r="385">
       <c r="A385" t="n">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="B385" t="inlineStr">
         <is>
-          <t>L1_CDC_SingleMu_3_er1p2_TOP120_DPHI2p618_3p142</t>
+          <t>L1_BPTX_BeamGas_B2_VME</t>
         </is>
       </c>
       <c r="C385" t="n">
         <v>0</v>
       </c>
       <c r="D385" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E385" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="F385" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="G385" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="H385" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="I385" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="J385" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="K385" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="386">
       <c r="A386" t="n">
-        <v>500</v>
+        <v>494</v>
       </c>
       <c r="B386" t="inlineStr">
         <is>
-          <t>L1_HCAL_LaserMon_Trig</t>
+          <t>L1_CDC_SingleMu_3_er1p2_TOP120_DPHI2p618_3p142</t>
         </is>
       </c>
       <c r="C386" t="n">
         <v>0</v>
       </c>
       <c r="D386" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E386" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="F386" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="G386" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H386" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="I386" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="J386" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="K386" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="387">
       <c r="A387" t="n">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="B387" t="inlineStr">
         <is>
-          <t>L1_HCAL_LaserMon_Veto</t>
+          <t>L1_HCAL_LaserMon_Trig</t>
         </is>
       </c>
       <c r="C387" t="n">
@@ -14774,11 +14774,11 @@
     </row>
     <row r="388">
       <c r="A388" t="n">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="B388" t="inlineStr">
         <is>
-          <t>L1_TOTEM_1</t>
+          <t>L1_HCAL_LaserMon_Veto</t>
         </is>
       </c>
       <c r="C388" t="n">
@@ -14811,11 +14811,11 @@
     </row>
     <row r="389">
       <c r="A389" t="n">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="B389" t="inlineStr">
         <is>
-          <t>L1_TOTEM_2</t>
+          <t>L1_TOTEM_1</t>
         </is>
       </c>
       <c r="C389" t="n">
@@ -14848,11 +14848,11 @@
     </row>
     <row r="390">
       <c r="A390" t="n">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="B390" t="inlineStr">
         <is>
-          <t>L1_TOTEM_3</t>
+          <t>L1_TOTEM_2</t>
         </is>
       </c>
       <c r="C390" t="n">
@@ -14885,38 +14885,75 @@
     </row>
     <row r="391">
       <c r="A391" t="n">
+        <v>505</v>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t>L1_TOTEM_3</t>
+        </is>
+      </c>
+      <c r="C391" t="n">
+        <v>0</v>
+      </c>
+      <c r="D391" t="n">
+        <v>0</v>
+      </c>
+      <c r="E391" t="n">
+        <v>0</v>
+      </c>
+      <c r="F391" t="n">
+        <v>0</v>
+      </c>
+      <c r="G391" t="n">
+        <v>0</v>
+      </c>
+      <c r="H391" t="n">
+        <v>0</v>
+      </c>
+      <c r="I391" t="n">
+        <v>0</v>
+      </c>
+      <c r="J391" t="n">
+        <v>0</v>
+      </c>
+      <c r="K391" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="n">
         <v>506</v>
       </c>
-      <c r="B391" t="inlineStr">
+      <c r="B392" t="inlineStr">
         <is>
           <t>L1_TOTEM_4</t>
         </is>
       </c>
-      <c r="C391" t="n">
-        <v>0</v>
-      </c>
-      <c r="D391" t="n">
-        <v>0</v>
-      </c>
-      <c r="E391" t="n">
-        <v>0</v>
-      </c>
-      <c r="F391" t="n">
-        <v>0</v>
-      </c>
-      <c r="G391" t="n">
-        <v>0</v>
-      </c>
-      <c r="H391" t="n">
-        <v>0</v>
-      </c>
-      <c r="I391" t="n">
-        <v>0</v>
-      </c>
-      <c r="J391" t="n">
-        <v>0</v>
-      </c>
-      <c r="K391" t="n">
+      <c r="C392" t="n">
+        <v>0</v>
+      </c>
+      <c r="D392" t="n">
+        <v>0</v>
+      </c>
+      <c r="E392" t="n">
+        <v>0</v>
+      </c>
+      <c r="F392" t="n">
+        <v>0</v>
+      </c>
+      <c r="G392" t="n">
+        <v>0</v>
+      </c>
+      <c r="H392" t="n">
+        <v>0</v>
+      </c>
+      <c r="I392" t="n">
+        <v>0</v>
+      </c>
+      <c r="J392" t="n">
+        <v>0</v>
+      </c>
+      <c r="K392" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
adding PS tables for LLP seeds grouped together menu
</commit_message>
<xml_diff>
--- a/development/L1Menu_Collisions2022_v1_1_0/PrescaleTable/L1Menu_Collisions2022_v1_1_0.xlsx
+++ b/development/L1Menu_Collisions2022_v1_1_0/PrescaleTable/L1Menu_Collisions2022_v1_1_0.xlsx
@@ -10815,270 +10815,270 @@
     </row>
     <row r="281">
       <c r="A281" t="n">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="B281" t="inlineStr">
         <is>
-          <t>L1_DoubleLLPJet40</t>
+          <t>L1_DoubleJet40er2p5</t>
         </is>
       </c>
       <c r="C281" t="n">
         <v>0</v>
       </c>
       <c r="D281" t="n">
-        <v>0</v>
+        <v>8400</v>
       </c>
       <c r="E281" t="n">
-        <v>0</v>
+        <v>8400</v>
       </c>
       <c r="F281" t="n">
-        <v>0</v>
+        <v>8400</v>
       </c>
       <c r="G281" t="n">
-        <v>0</v>
+        <v>8400</v>
       </c>
       <c r="H281" t="n">
-        <v>0</v>
+        <v>8400</v>
       </c>
       <c r="I281" t="n">
-        <v>0</v>
+        <v>8400</v>
       </c>
       <c r="J281" t="n">
-        <v>0</v>
+        <v>8400</v>
       </c>
       <c r="K281" t="n">
-        <v>0</v>
+        <v>8400</v>
       </c>
     </row>
     <row r="282">
       <c r="A282" t="n">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="B282" t="inlineStr">
         <is>
-          <t>L1_DoubleJet40er2p5</t>
+          <t>L1_DoubleJet100er2p5</t>
         </is>
       </c>
       <c r="C282" t="n">
         <v>0</v>
       </c>
       <c r="D282" t="n">
-        <v>8400</v>
+        <v>170</v>
       </c>
       <c r="E282" t="n">
-        <v>8400</v>
+        <v>170</v>
       </c>
       <c r="F282" t="n">
-        <v>8400</v>
+        <v>170</v>
       </c>
       <c r="G282" t="n">
-        <v>8400</v>
+        <v>170</v>
       </c>
       <c r="H282" t="n">
-        <v>8400</v>
+        <v>170</v>
       </c>
       <c r="I282" t="n">
-        <v>8400</v>
+        <v>170</v>
       </c>
       <c r="J282" t="n">
-        <v>8400</v>
+        <v>170</v>
       </c>
       <c r="K282" t="n">
-        <v>8400</v>
+        <v>170</v>
       </c>
     </row>
     <row r="283">
       <c r="A283" t="n">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="B283" t="inlineStr">
         <is>
-          <t>L1_DoubleJet100er2p5</t>
+          <t>L1_DoubleJet120er2p5</t>
         </is>
       </c>
       <c r="C283" t="n">
         <v>0</v>
       </c>
       <c r="D283" t="n">
-        <v>170</v>
+        <v>70</v>
       </c>
       <c r="E283" t="n">
-        <v>170</v>
+        <v>70</v>
       </c>
       <c r="F283" t="n">
-        <v>170</v>
+        <v>70</v>
       </c>
       <c r="G283" t="n">
-        <v>170</v>
+        <v>70</v>
       </c>
       <c r="H283" t="n">
-        <v>170</v>
+        <v>70</v>
       </c>
       <c r="I283" t="n">
-        <v>170</v>
+        <v>70</v>
       </c>
       <c r="J283" t="n">
-        <v>170</v>
+        <v>70</v>
       </c>
       <c r="K283" t="n">
-        <v>170</v>
+        <v>70</v>
       </c>
     </row>
     <row r="284">
       <c r="A284" t="n">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="B284" t="inlineStr">
         <is>
-          <t>L1_DoubleJet120er2p5</t>
+          <t>L1_DoubleJet150er2p5</t>
         </is>
       </c>
       <c r="C284" t="n">
         <v>0</v>
       </c>
       <c r="D284" t="n">
-        <v>70</v>
+        <v>1</v>
       </c>
       <c r="E284" t="n">
-        <v>70</v>
+        <v>1</v>
       </c>
       <c r="F284" t="n">
-        <v>70</v>
+        <v>1</v>
       </c>
       <c r="G284" t="n">
-        <v>70</v>
+        <v>1</v>
       </c>
       <c r="H284" t="n">
-        <v>70</v>
+        <v>1</v>
       </c>
       <c r="I284" t="n">
-        <v>70</v>
+        <v>1</v>
       </c>
       <c r="J284" t="n">
-        <v>70</v>
+        <v>1</v>
       </c>
       <c r="K284" t="n">
-        <v>70</v>
+        <v>1</v>
       </c>
     </row>
     <row r="285">
       <c r="A285" t="n">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="B285" t="inlineStr">
         <is>
-          <t>L1_DoubleJet150er2p5</t>
+          <t>L1_DoubleJet100er2p3_dEta_Max1p6</t>
         </is>
       </c>
       <c r="C285" t="n">
         <v>0</v>
       </c>
       <c r="D285" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E285" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F285" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G285" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H285" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I285" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J285" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K285" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="286">
       <c r="A286" t="n">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B286" t="inlineStr">
         <is>
-          <t>L1_DoubleJet100er2p3_dEta_Max1p6</t>
+          <t>L1_DoubleJet112er2p3_dEta_Max1p6</t>
         </is>
       </c>
       <c r="C286" t="n">
         <v>0</v>
       </c>
       <c r="D286" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E286" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F286" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G286" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H286" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I286" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J286" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K286" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="287">
       <c r="A287" t="n">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="B287" t="inlineStr">
         <is>
-          <t>L1_DoubleJet112er2p3_dEta_Max1p6</t>
+          <t>L1_DoubleJet30er2p5_Mass_Min150_dEta_Max1p5</t>
         </is>
       </c>
       <c r="C287" t="n">
         <v>0</v>
       </c>
       <c r="D287" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E287" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F287" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G287" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H287" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I287" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J287" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K287" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="288">
       <c r="A288" t="n">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="B288" t="inlineStr">
         <is>
-          <t>L1_DoubleJet30er2p5_Mass_Min150_dEta_Max1p5</t>
+          <t>L1_DoubleJet30er2p5_Mass_Min200_dEta_Max1p5</t>
         </is>
       </c>
       <c r="C288" t="n">
@@ -11111,11 +11111,11 @@
     </row>
     <row r="289">
       <c r="A289" t="n">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="B289" t="inlineStr">
         <is>
-          <t>L1_DoubleJet30er2p5_Mass_Min200_dEta_Max1p5</t>
+          <t>L1_DoubleJet30er2p5_Mass_Min250_dEta_Max1p5</t>
         </is>
       </c>
       <c r="C289" t="n">
@@ -11148,48 +11148,48 @@
     </row>
     <row r="290">
       <c r="A290" t="n">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B290" t="inlineStr">
         <is>
-          <t>L1_DoubleJet30er2p5_Mass_Min250_dEta_Max1p5</t>
+          <t>L1_DoubleJet30er2p5_Mass_Min300_dEta_Max1p5</t>
         </is>
       </c>
       <c r="C290" t="n">
         <v>0</v>
       </c>
       <c r="D290" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E290" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F290" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G290" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H290" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I290" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J290" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K290" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="291">
       <c r="A291" t="n">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="B291" t="inlineStr">
         <is>
-          <t>L1_DoubleJet30er2p5_Mass_Min300_dEta_Max1p5</t>
+          <t>L1_DoubleJet30er2p5_Mass_Min330_dEta_Max1p5</t>
         </is>
       </c>
       <c r="C291" t="n">
@@ -11222,11 +11222,11 @@
     </row>
     <row r="292">
       <c r="A292" t="n">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="B292" t="inlineStr">
         <is>
-          <t>L1_DoubleJet30er2p5_Mass_Min330_dEta_Max1p5</t>
+          <t>L1_DoubleJet30er2p5_Mass_Min360_dEta_Max1p5</t>
         </is>
       </c>
       <c r="C292" t="n">
@@ -11259,48 +11259,48 @@
     </row>
     <row r="293">
       <c r="A293" t="n">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="B293" t="inlineStr">
         <is>
-          <t>L1_DoubleJet30er2p5_Mass_Min360_dEta_Max1p5</t>
+          <t>L1_DoubleJet_90_30_DoubleJet30_Mass_Min620</t>
         </is>
       </c>
       <c r="C293" t="n">
         <v>0</v>
       </c>
       <c r="D293" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E293" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F293" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G293" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H293" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I293" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J293" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K293" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="294">
       <c r="A294" t="n">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="B294" t="inlineStr">
         <is>
-          <t>L1_DoubleJet_90_30_DoubleJet30_Mass_Min620</t>
+          <t>L1_DoubleJet_100_30_DoubleJet30_Mass_Min620</t>
         </is>
       </c>
       <c r="C294" t="n">
@@ -11333,11 +11333,11 @@
     </row>
     <row r="295">
       <c r="A295" t="n">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="B295" t="inlineStr">
         <is>
-          <t>L1_DoubleJet_100_30_DoubleJet30_Mass_Min620</t>
+          <t>L1_DoubleJet_110_35_DoubleJet35_Mass_Min620</t>
         </is>
       </c>
       <c r="C295" t="n">
@@ -11347,41 +11347,41 @@
         <v>0</v>
       </c>
       <c r="E295" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F295" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G295" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H295" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I295" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J295" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K295" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="296">
       <c r="A296" t="n">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="B296" t="inlineStr">
         <is>
-          <t>L1_DoubleJet_110_35_DoubleJet35_Mass_Min620</t>
+          <t>L1_DoubleJet_115_40_DoubleJet40_Mass_Min620</t>
         </is>
       </c>
       <c r="C296" t="n">
         <v>0</v>
       </c>
       <c r="D296" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E296" t="n">
         <v>1</v>
@@ -11407,11 +11407,11 @@
     </row>
     <row r="297">
       <c r="A297" t="n">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="B297" t="inlineStr">
         <is>
-          <t>L1_DoubleJet_115_40_DoubleJet40_Mass_Min620</t>
+          <t>L1_DoubleJet_120_45_DoubleJet45_Mass_Min620</t>
         </is>
       </c>
       <c r="C297" t="n">
@@ -11444,11 +11444,11 @@
     </row>
     <row r="298">
       <c r="A298" t="n">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="B298" t="inlineStr">
         <is>
-          <t>L1_DoubleJet_120_45_DoubleJet45_Mass_Min620</t>
+          <t>L1_DoubleJet_115_40_DoubleJet40_Mass_Min620_Jet60TT28</t>
         </is>
       </c>
       <c r="C298" t="n">
@@ -11481,11 +11481,11 @@
     </row>
     <row r="299">
       <c r="A299" t="n">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="B299" t="inlineStr">
         <is>
-          <t>L1_DoubleJet_115_40_DoubleJet40_Mass_Min620_Jet60TT28</t>
+          <t>L1_DoubleJet_120_45_DoubleJet45_Mass_Min620_Jet60TT28</t>
         </is>
       </c>
       <c r="C299" t="n">
@@ -11518,48 +11518,48 @@
     </row>
     <row r="300">
       <c r="A300" t="n">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="B300" t="inlineStr">
         <is>
-          <t>L1_DoubleJet_120_45_DoubleJet45_Mass_Min620_Jet60TT28</t>
+          <t>L1_DoubleJet35_Mass_Min450_IsoTau45er2p1_RmOvlp_dR0p5</t>
         </is>
       </c>
       <c r="C300" t="n">
         <v>0</v>
       </c>
       <c r="D300" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E300" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F300" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G300" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H300" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I300" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J300" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K300" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="301">
       <c r="A301" t="n">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="B301" t="inlineStr">
         <is>
-          <t>L1_DoubleJet35_Mass_Min450_IsoTau45er2p1_RmOvlp_dR0p5</t>
+          <t>L1_DoubleJet35_Mass_Min450_IsoTau45_RmOvlp</t>
         </is>
       </c>
       <c r="C301" t="n">
@@ -11592,11 +11592,11 @@
     </row>
     <row r="302">
       <c r="A302" t="n">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="B302" t="inlineStr">
         <is>
-          <t>L1_DoubleJet35_Mass_Min450_IsoTau45_RmOvlp</t>
+          <t>L1_DoubleJet_80_30_Mass_Min420_IsoTau40_RmOvlp</t>
         </is>
       </c>
       <c r="C302" t="n">
@@ -11629,11 +11629,11 @@
     </row>
     <row r="303">
       <c r="A303" t="n">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="B303" t="inlineStr">
         <is>
-          <t>L1_DoubleJet_80_30_Mass_Min420_IsoTau40_RmOvlp</t>
+          <t>L1_DoubleJet_80_30_Mass_Min420_Mu8</t>
         </is>
       </c>
       <c r="C303" t="n">
@@ -11666,11 +11666,11 @@
     </row>
     <row r="304">
       <c r="A304" t="n">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="B304" t="inlineStr">
         <is>
-          <t>L1_DoubleJet_80_30_Mass_Min420_Mu8</t>
+          <t>L1_DoubleJet_80_30_Mass_Min420_DoubleMu0_SQ</t>
         </is>
       </c>
       <c r="C304" t="n">
@@ -11703,11 +11703,11 @@
     </row>
     <row r="305">
       <c r="A305" t="n">
-        <v>366</v>
+        <v>372</v>
       </c>
       <c r="B305" t="inlineStr">
         <is>
-          <t>L1_DoubleJet_80_30_Mass_Min420_DoubleMu0_SQ</t>
+          <t>L1_TripleJet_95_75_65_DoubleJet_75_65_er2p5</t>
         </is>
       </c>
       <c r="C305" t="n">
@@ -11717,41 +11717,41 @@
         <v>0</v>
       </c>
       <c r="E305" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F305" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G305" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H305" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I305" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J305" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K305" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="306">
       <c r="A306" t="n">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="B306" t="inlineStr">
         <is>
-          <t>L1_TripleJet_95_75_65_DoubleJet_75_65_er2p5</t>
+          <t>L1_TripleJet_100_80_70_DoubleJet_80_70_er2p5</t>
         </is>
       </c>
       <c r="C306" t="n">
         <v>0</v>
       </c>
       <c r="D306" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E306" t="n">
         <v>1</v>
@@ -11777,11 +11777,11 @@
     </row>
     <row r="307">
       <c r="A307" t="n">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="B307" t="inlineStr">
         <is>
-          <t>L1_TripleJet_100_80_70_DoubleJet_80_70_er2p5</t>
+          <t>L1_TripleJet_105_85_75_DoubleJet_85_75_er2p5</t>
         </is>
       </c>
       <c r="C307" t="n">
@@ -11814,11 +11814,11 @@
     </row>
     <row r="308">
       <c r="A308" t="n">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="B308" t="inlineStr">
         <is>
-          <t>L1_TripleJet_105_85_75_DoubleJet_85_75_er2p5</t>
+          <t>L1_QuadJet_95_75_65_20_DoubleJet_75_65_er2p5_Jet20_FWD3p0</t>
         </is>
       </c>
       <c r="C308" t="n">
@@ -11851,48 +11851,48 @@
     </row>
     <row r="309">
       <c r="A309" t="n">
-        <v>376</v>
+        <v>382</v>
       </c>
       <c r="B309" t="inlineStr">
         <is>
-          <t>L1_QuadJet_95_75_65_20_DoubleJet_75_65_er2p5_Jet20_FWD3p0</t>
+          <t>L1_QuadJet60er2p5</t>
         </is>
       </c>
       <c r="C309" t="n">
         <v>0</v>
       </c>
       <c r="D309" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E309" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F309" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G309" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H309" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I309" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J309" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K309" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="310">
       <c r="A310" t="n">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="B310" t="inlineStr">
         <is>
-          <t>L1_QuadJet60er2p5</t>
+          <t>L1_HTT120_SingleLLPJet40</t>
         </is>
       </c>
       <c r="C310" t="n">
@@ -11929,7 +11929,7 @@
       </c>
       <c r="B311" t="inlineStr">
         <is>
-          <t>L1_HTT280er_QuadJet_70_55_40_35_er2p5</t>
+          <t>L1_HTT160_SingleLLPJet50</t>
         </is>
       </c>
       <c r="C311" t="n">
@@ -11966,7 +11966,7 @@
       </c>
       <c r="B312" t="inlineStr">
         <is>
-          <t>L1_HTT320er_QuadJet_70_55_40_40_er2p5</t>
+          <t>L1_HTT200_SingleLLPJet60</t>
         </is>
       </c>
       <c r="C312" t="n">
@@ -11976,25 +11976,25 @@
         <v>0</v>
       </c>
       <c r="E312" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F312" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G312" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H312" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I312" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J312" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K312" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="313">
@@ -12003,35 +12003,35 @@
       </c>
       <c r="B313" t="inlineStr">
         <is>
-          <t>L1_HTT320er_QuadJet_80_60_er2p1_45_40_er2p3</t>
+          <t>L1_HTT240_SingleLLPJet70</t>
         </is>
       </c>
       <c r="C313" t="n">
         <v>0</v>
       </c>
       <c r="D313" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E313" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F313" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G313" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H313" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I313" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J313" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K313" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="314">
@@ -12040,35 +12040,35 @@
       </c>
       <c r="B314" t="inlineStr">
         <is>
-          <t>L1_HTT320er_QuadJet_80_60_er2p1_50_45_er2p3</t>
+          <t>L1_DoubleLLPJet40</t>
         </is>
       </c>
       <c r="C314" t="n">
         <v>0</v>
       </c>
       <c r="D314" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E314" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F314" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G314" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H314" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I314" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J314" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K314" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="315">
@@ -12077,7 +12077,7 @@
       </c>
       <c r="B315" t="inlineStr">
         <is>
-          <t>L1_HTT120_SingleLLPJet40</t>
+          <t>L1_HTT280er_QuadJet_70_55_40_35_er2p5</t>
         </is>
       </c>
       <c r="C315" t="n">
@@ -12114,7 +12114,7 @@
       </c>
       <c r="B316" t="inlineStr">
         <is>
-          <t>L1_HTT160_SingleLLPJet50</t>
+          <t>L1_HTT320er_QuadJet_70_55_40_40_er2p5</t>
         </is>
       </c>
       <c r="C316" t="n">
@@ -12124,25 +12124,25 @@
         <v>0</v>
       </c>
       <c r="E316" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F316" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G316" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H316" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I316" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J316" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K316" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="317">
@@ -12151,35 +12151,35 @@
       </c>
       <c r="B317" t="inlineStr">
         <is>
-          <t>L1_HTT200_SingleLLPJet60</t>
+          <t>L1_HTT320er_QuadJet_80_60_er2p1_45_40_er2p3</t>
         </is>
       </c>
       <c r="C317" t="n">
         <v>0</v>
       </c>
       <c r="D317" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E317" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F317" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G317" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H317" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I317" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J317" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K317" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="318">
@@ -12188,35 +12188,35 @@
       </c>
       <c r="B318" t="inlineStr">
         <is>
-          <t>L1_HTT240_SingleLLPJet70</t>
+          <t>L1_HTT320er_QuadJet_80_60_er2p1_50_45_er2p3</t>
         </is>
       </c>
       <c r="C318" t="n">
         <v>0</v>
       </c>
       <c r="D318" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E318" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F318" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G318" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H318" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I318" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J318" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K318" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="319">

</xml_diff>

<commit_message>
fixing the LLPDoubleJet place
</commit_message>
<xml_diff>
--- a/development/L1Menu_Collisions2022_v1_1_0/PrescaleTable/L1Menu_Collisions2022_v1_1_0.xlsx
+++ b/development/L1Menu_Collisions2022_v1_1_0/PrescaleTable/L1Menu_Collisions2022_v1_1_0.xlsx
@@ -11892,7 +11892,7 @@
       </c>
       <c r="B310" t="inlineStr">
         <is>
-          <t>L1_HTT120_SingleLLPJet40</t>
+          <t>L1_DoubleLLPJet40</t>
         </is>
       </c>
       <c r="C310" t="n">
@@ -11929,7 +11929,7 @@
       </c>
       <c r="B311" t="inlineStr">
         <is>
-          <t>L1_HTT160_SingleLLPJet50</t>
+          <t>L1_HTT120_SingleLLPJet40</t>
         </is>
       </c>
       <c r="C311" t="n">
@@ -11966,7 +11966,7 @@
       </c>
       <c r="B312" t="inlineStr">
         <is>
-          <t>L1_HTT200_SingleLLPJet60</t>
+          <t>L1_HTT160_SingleLLPJet50</t>
         </is>
       </c>
       <c r="C312" t="n">
@@ -12003,7 +12003,7 @@
       </c>
       <c r="B313" t="inlineStr">
         <is>
-          <t>L1_HTT240_SingleLLPJet70</t>
+          <t>L1_HTT200_SingleLLPJet60</t>
         </is>
       </c>
       <c r="C313" t="n">
@@ -12040,7 +12040,7 @@
       </c>
       <c r="B314" t="inlineStr">
         <is>
-          <t>L1_DoubleLLPJet40</t>
+          <t>L1_HTT240_SingleLLPJet70</t>
         </is>
       </c>
       <c r="C314" t="n">

</xml_diff>